<commit_message>
added yet more changes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13760" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Profit</t>
   </si>
@@ -48,6 +49,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -365,7 +369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +447,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>